<commit_message>
Modify: fix the candidate seeder
</commit_message>
<xml_diff>
--- a/storage/app/candidate.xlsx
+++ b/storage/app/candidate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D7C98F-E06E-48D0-89E0-4500D6A1AD8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E161AD72-145F-4CFC-9D77-389890B2FEF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="3330" windowWidth="9660" windowHeight="6210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baza Uczestników 02.04.2021 — A" sheetId="1" r:id="rId1"/>
@@ -9277,9 +9277,6 @@
     <t>ZUS Zielona Góra</t>
   </si>
   <si>
-    <t>M1-W-022</t>
-  </si>
-  <si>
     <t>Igor Kosowicz</t>
   </si>
   <si>
@@ -9287,6 +9284,9 @@
   </si>
   <si>
     <t>05-05-2021</t>
+  </si>
+  <si>
+    <t>M1-W022</t>
   </si>
 </sst>
 </file>
@@ -10354,8 +10354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF548"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A520" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H537" sqref="H537"/>
+    <sheetView tabSelected="1" topLeftCell="O13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12717,7 +12717,7 @@
         <v>2687</v>
       </c>
       <c r="V26" s="4" t="s">
-        <v>3085</v>
+        <v>3088</v>
       </c>
       <c r="W26" s="4" t="s">
         <v>38</v>
@@ -56190,7 +56190,7 @@
         <v>52</v>
       </c>
       <c r="AB541" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC541" s="4" t="s">
         <v>71</v>
@@ -56270,7 +56270,7 @@
         <v>52</v>
       </c>
       <c r="AB542" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC542" s="4" t="s">
         <v>71</v>
@@ -56348,7 +56348,7 @@
         <v>52</v>
       </c>
       <c r="AB543" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC543" s="4" t="s">
         <v>71</v>
@@ -56424,7 +56424,7 @@
         <v>52</v>
       </c>
       <c r="AB544" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC544" s="4" t="s">
         <v>71</v>
@@ -56502,7 +56502,7 @@
         <v>38</v>
       </c>
       <c r="AB545" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC545" s="4" t="s">
         <v>327</v>
@@ -56578,7 +56578,7 @@
         <v>38</v>
       </c>
       <c r="AB546" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC546" s="4" t="s">
         <v>327</v>
@@ -56644,19 +56644,19 @@
         <v>38</v>
       </c>
       <c r="X547" s="4" t="s">
+        <v>3085</v>
+      </c>
+      <c r="Y547" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z547" s="21" t="s">
         <v>3086</v>
       </c>
-      <c r="Y547" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z547" s="21" t="s">
+      <c r="AA547" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB547" s="36" t="s">
         <v>3087</v>
-      </c>
-      <c r="AA547" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB547" s="36" t="s">
-        <v>3088</v>
       </c>
       <c r="AC547" s="4" t="s">
         <v>327</v>
@@ -56730,7 +56730,7 @@
         <v>52</v>
       </c>
       <c r="AB548" s="36" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="AC548" s="4" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Modify: change the candidate seeder
</commit_message>
<xml_diff>
--- a/storage/app/candidate.xlsx
+++ b/storage/app/candidate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3866C18-8EFD-4F10-A9F1-05E3E4B34B6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D24156-22A2-4110-AD9E-A100F57AEF90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="8370" windowWidth="9660" windowHeight="6210" xr2:uid="{8D55E213-DD71-459B-A4FB-03542688079A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8D55E213-DD71-459B-A4FB-03542688079A}"/>
   </bookViews>
   <sheets>
     <sheet name="baza" sheetId="1" r:id="rId1"/>
@@ -9419,13 +9419,13 @@
     <t>Nodzykowska</t>
   </si>
   <si>
-    <t>employ_status_1</t>
-  </si>
-  <si>
     <t>5x10x2021</t>
   </si>
   <si>
     <t>13-05-2021</t>
+  </si>
+  <si>
+    <t>employ_status1</t>
   </si>
 </sst>
 </file>
@@ -10194,10 +10194,10 @@
   <dimension ref="A1:AF550"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Z542" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G542" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE545" sqref="AE545"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10290,7 +10290,7 @@
         <v>2935</v>
       </c>
       <c r="R1" s="104" t="s">
-        <v>3129</v>
+        <v>3131</v>
       </c>
       <c r="S1" s="109" t="s">
         <v>2921</v>
@@ -58446,7 +58446,7 @@
       <c r="O549" s="86"/>
       <c r="P549" s="91"/>
       <c r="Q549" s="97" t="s">
-        <v>3130</v>
+        <v>3129</v>
       </c>
       <c r="R549" s="99"/>
       <c r="S549" s="106"/>
@@ -58469,7 +58469,7 @@
         <v>1303</v>
       </c>
       <c r="AC549" s="160" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
       <c r="AD549" s="161"/>
     </row>
@@ -58495,7 +58495,7 @@
       <c r="O550" s="86"/>
       <c r="P550" s="91"/>
       <c r="Q550" s="97" t="s">
-        <v>3130</v>
+        <v>3129</v>
       </c>
       <c r="R550" s="99"/>
       <c r="S550" s="106"/>
@@ -58518,7 +58518,7 @@
         <v>1420</v>
       </c>
       <c r="AC550" s="160" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
       <c r="AD550" s="161"/>
     </row>

</xml_diff>